<commit_message>
added test for excel
Signed-off-by: Zehra Ciftci <CiftciZ@rki.de>
</commit_message>
<xml_diff>
--- a/tests/test_files/test.xlsx
+++ b/tests/test_files/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciftciz\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Repos\mex-drop\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4195423A-4018-4EF2-9DF8-1111F058F315}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7A28A0-FAF2-4E68-BF07-00C946C6698E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10395" xr2:uid="{E5132201-2820-45A6-A107-C69699E5BE72}"/>
   </bookViews>
@@ -40,10 +40,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,8 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -385,28 +393,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13B4559-03CB-449F-BCA3-B19CFDEB8463}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>